<commit_message>
updates with reviewed points
</commit_message>
<xml_diff>
--- a/Results/AreasofDisturbance_ceoV3version_SAVE.xlsx
+++ b/Results/AreasofDisturbance_ceoV3version_SAVE.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,29 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e0c35774a9514c4a/Documents/Philippines/PhilippinesQAQCanalysis/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B057B23D-3323-4E4B-9013-E14C68BF025F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="8_{9954C90C-C671-43EA-AEFF-5C1010FD1291}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9D0A3913-6D4D-4531-B20F-E2345C697F94}"/>
   <bookViews>
-    <workbookView xWindow="62905" yWindow="1255" windowWidth="23495" windowHeight="11340"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AreasofDisturbance_ceoV3version" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>Total, ha</t>
   </si>
@@ -28,36 +38,46 @@
     <t>SE, ha</t>
   </si>
   <si>
-    <t>CEOreadable_v3Deforestation</t>
+    <t>Deforestation</t>
   </si>
   <si>
-    <t>CEOreadable_v3Degradation</t>
+    <t>Degradation</t>
   </si>
   <si>
-    <t>CEOreadable_v3multiple events</t>
+    <t>multiple events</t>
   </si>
   <si>
-    <t>CEOreadable_v3Reforestation</t>
+    <t>Reforestation</t>
   </si>
   <si>
-    <t>CEOreadable_v3stable forest</t>
+    <t>stable forest</t>
   </si>
   <si>
-    <t>CEOreadable_v3stable non forest</t>
+    <t>stable non-forest</t>
   </si>
   <si>
-    <t>weight</t>
+    <t>stable non forest</t>
   </si>
   <si>
-    <t>SE/area</t>
+    <t>relative difference</t>
+  </si>
+  <si>
+    <t>(mapped-estimated)/estimated</t>
+  </si>
+  <si>
+    <t>deforested</t>
+  </si>
+  <si>
+    <t>map area, ha</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.0%"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -376,7 +396,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -491,10 +511,89 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -536,55 +635,67 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="42" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="14" xfId="43" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="42" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="17" xfId="43" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="43">
-    <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="24" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="28" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="32" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="36" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="40" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="21" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="25" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="29" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="33" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="37" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="41" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="22" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="26" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="30" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="34" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="38" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="42" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="19" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="23" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="27" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="31" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="35" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="39" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="8" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="12" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="14" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="17" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="7" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="3" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="4" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="5" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="6" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="10" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="13" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="9" builtinId="28" customBuiltin="1"/>
+  <cellStyles count="44">
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Comma" xfId="42" builtinId="3"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="16" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="11" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
-    <cellStyle name="Title" xfId="2" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="18" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="15" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Percent" xfId="43" builtinId="5"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -597,6 +708,1810 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>AreasofDisturbance_ceoV3version!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total, ha</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>AreasofDisturbance_ceoV3version!$A$2:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Deforestation</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Degradation</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>multiple events</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Reforestation</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>stable forest</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>stable non-forest</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>AreasofDisturbance_ceoV3version!$B$2:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>907377</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>739801</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>208200</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>696393</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8093184</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>19091373</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3D44-47B8-BF3A-4EA942C76895}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>AreasofDisturbance_ceoV3version!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>map area, ha</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>AreasofDisturbance_ceoV3version!$A$2:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Deforestation</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Degradation</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>multiple events</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Reforestation</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>stable forest</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>stable non-forest</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>AreasofDisturbance_ceoV3version!$D$2:$D$7</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>3100835.07</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3440705.22</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2397981.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7458958.7999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13337846.91</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0EE3-4C04-AEB7-1807DE3A67C4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>22225</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>15875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>155575</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA2E2295-FCCB-4A3C-9A89-63B5E140EAC4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>182562</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>182562</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C0E3BFF-ECAA-4921-B28A-5B2BF5FEBCF4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -895,144 +2810,200 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <cols>
+    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="2" max="2" width="19.76953125" customWidth="1"/>
+    <col min="3" max="3" width="10.86328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.08984375" customWidth="1"/>
+    <col min="5" max="5" width="26.7265625" customWidth="1"/>
+    <col min="10" max="10" width="18.86328125" customWidth="1"/>
+    <col min="11" max="11" width="17.6328125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="B1" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A1" s="2"/>
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E1" t="s">
+      <c r="I1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1">
+        <v>34453723</v>
+      </c>
+      <c r="K1" s="1">
+        <f>J1*30*30/10000</f>
+        <v>3100835.07</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="6">
+        <v>907377</v>
+      </c>
+      <c r="C2" s="6">
+        <v>161195</v>
+      </c>
+      <c r="D2" s="6">
+        <v>3100835.07</v>
+      </c>
+      <c r="E2" s="7">
+        <f>(D2-B2)/B2</f>
+        <v>2.4173613283122668</v>
+      </c>
+      <c r="I2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2">
+        <v>38230058</v>
+      </c>
+      <c r="K2" s="1">
+        <f>J2*30*30/10000</f>
+        <v>3440705.22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="6">
+        <v>739801</v>
+      </c>
+      <c r="C3" s="6">
+        <v>144576</v>
+      </c>
+      <c r="D3" s="6"/>
+      <c r="E3" s="7"/>
+      <c r="I3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J3">
+        <v>26644240</v>
+      </c>
+      <c r="K3" s="1">
+        <f t="shared" ref="K3:K4" si="0">J3*30*30/10000</f>
+        <v>2397981.6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="6">
+        <v>208200</v>
+      </c>
+      <c r="C4" s="6">
+        <v>73025</v>
+      </c>
+      <c r="D4" s="6">
+        <v>3440705.22</v>
+      </c>
+      <c r="E4" s="7">
+        <f t="shared" ref="E4:E7" si="1">(D4-B4)/B4</f>
+        <v>15.525961671469741</v>
+      </c>
+      <c r="I4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J4">
+        <v>82877320</v>
+      </c>
+      <c r="K4" s="1">
+        <f t="shared" si="0"/>
+        <v>7458958.7999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="6">
+        <v>696393</v>
+      </c>
+      <c r="C5" s="6">
+        <v>131442</v>
+      </c>
+      <c r="D5" s="6">
+        <v>2397981.6</v>
+      </c>
+      <c r="E5" s="7">
+        <f t="shared" si="1"/>
+        <v>2.4434315106556213</v>
+      </c>
+      <c r="I5" t="s">
         <v>8</v>
       </c>
+      <c r="J5">
+        <v>148198299</v>
+      </c>
+      <c r="K5" s="1">
+        <f>J5*30*30/10000</f>
+        <v>13337846.91</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2">
-        <v>789342</v>
-      </c>
-      <c r="C2">
-        <v>148691</v>
-      </c>
-      <c r="D2" s="1">
-        <f>C2/B2</f>
-        <v>0.188373354008782</v>
-      </c>
-      <c r="E2" s="1">
-        <f>B2/SUM(B$2:B$7)</f>
-        <v>2.9249059516575419E-2</v>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="6">
+        <v>8093184</v>
+      </c>
+      <c r="C6" s="6">
+        <v>306120</v>
+      </c>
+      <c r="D6" s="6">
+        <v>7458958.7999999998</v>
+      </c>
+      <c r="E6" s="7">
+        <f t="shared" si="1"/>
+        <v>-7.8365350398557618E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>626518</v>
-      </c>
-      <c r="C3">
-        <v>131392</v>
-      </c>
-      <c r="D3" s="1">
-        <f t="shared" ref="D3:D7" si="0">C3/B3</f>
-        <v>0.20971783731672514</v>
-      </c>
-      <c r="E3" s="1">
-        <f t="shared" ref="E3:E7" si="1">B3/SUM(B$2:B$7)</f>
-        <v>2.321561790732762E-2</v>
+    <row r="7" spans="1:11" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="A7" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="9">
+        <v>19091373</v>
+      </c>
+      <c r="C7" s="9">
+        <v>325231</v>
+      </c>
+      <c r="D7" s="9">
+        <v>13337846.91</v>
+      </c>
+      <c r="E7" s="10">
+        <f t="shared" si="1"/>
+        <v>-0.30136785290403156</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4">
-        <v>169549</v>
-      </c>
-      <c r="C4">
-        <v>65958</v>
-      </c>
-      <c r="D4" s="1">
-        <f t="shared" si="0"/>
-        <v>0.38902028322195942</v>
-      </c>
-      <c r="E4" s="1">
-        <f t="shared" si="1"/>
-        <v>6.282636413589858E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>500201</v>
-      </c>
-      <c r="C5">
-        <v>109717</v>
-      </c>
-      <c r="D5" s="1">
-        <f t="shared" si="0"/>
-        <v>0.21934582297916239</v>
-      </c>
-      <c r="E5" s="1">
-        <f t="shared" si="1"/>
-        <v>1.8534942799509645E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6">
-        <v>7433206</v>
-      </c>
-      <c r="C6">
-        <v>281008</v>
-      </c>
-      <c r="D6" s="1">
-        <f t="shared" si="0"/>
-        <v>3.7804414407457562E-2</v>
-      </c>
-      <c r="E6" s="1">
-        <f t="shared" si="1"/>
-        <v>0.27543737023111087</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7">
-        <v>17468103</v>
-      </c>
-      <c r="C7">
-        <v>297680</v>
-      </c>
-      <c r="D7" s="1">
-        <f t="shared" si="0"/>
-        <v>1.7041346733529108E-2</v>
-      </c>
-      <c r="E7" s="1">
-        <f t="shared" si="1"/>
-        <v>0.64728037313188658</v>
-      </c>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="E9" t="s">
+        <v>10</v>
+      </c>
+      <c r="K9" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>